<commit_message>
kod zrobiony, to do komentarze
</commit_message>
<xml_diff>
--- a/dnd.xlsx
+++ b/dnd.xlsx
@@ -1,17 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
-  </bookViews>
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="class" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="race" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="character" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="dupa" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="dupaa" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -23,13 +21,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
       <b val="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,19 +45,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -74,9 +61,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -159,44 +146,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -226,12 +213,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -270,142 +257,201 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
+                <a:tint val="100000"/>
                 <a:shade val="100000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -418,17 +464,10 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12.7109375" customWidth="1" min="2" max="2"/>
-    <col width="10.7109375" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="10.5703125" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="9.85546875" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="10.42578125" bestFit="1" customWidth="1" min="6" max="7"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="B1" t="inlineStr">
@@ -522,7 +561,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -535,18 +574,10 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="17" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="9.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="10.7109375" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="10.5703125" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="9.85546875" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="10.42578125" bestFit="1" customWidth="1" min="6" max="7"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="B1" t="inlineStr">
@@ -586,23 +617,35 @@
           <t>dwarf(hill)</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -611,23 +654,35 @@
           <t>dwarf(mountain)</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -636,23 +691,35 @@
           <t>elf(high)</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -661,23 +728,35 @@
           <t>elf(wood)</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -686,23 +765,35 @@
           <t>elf(drow)</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -711,23 +802,35 @@
           <t>halfling(lightfoot)</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -736,23 +839,35 @@
           <t>halfling(stout)</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -761,23 +876,35 @@
           <t>human</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -786,23 +913,35 @@
           <t>dragonborn</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -811,23 +950,35 @@
           <t xml:space="preserve">gnome(forest)	</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>2</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -836,23 +987,35 @@
           <t xml:space="preserve">gnome(rock)	</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" t="n">
-        <v>2</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -861,23 +1024,35 @@
           <t>halfelf</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>2</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -886,23 +1061,35 @@
           <t>halforc</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -911,27 +1098,39 @@
           <t>tiefling</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="n">
-        <v>2</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -943,7 +1142,233 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Race</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Strength</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Dexterity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Constitution</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Intelligence</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Wisdom</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Charisma</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>hi</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>fighter</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>elf(drow)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Race</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Strength</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Dexterity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Constitution</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Intelligence</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Wisdom</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Charisma</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ranger</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>human, (STR: 1, DEX: 1, CON: 1, INT: 1, WIS: 1, CHA: 1)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -999,36 +1424,36 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>hi</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>fighter</t>
+          <t>cleric</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>elf(drow)</t>
+          <t>dwarf(hill)</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" t="n">
+        <v>14</v>
+      </c>
+      <c r="F2" t="n">
         <v>16</v>
       </c>
-      <c r="F2" t="n">
-        <v>13</v>
-      </c>
       <c r="G2" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H2" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="I2" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>